<commit_message>
hsv lab xyz yuv
</commit_message>
<xml_diff>
--- a/stage2_excels/GA/GA_color_space.xlsx
+++ b/stage2_excels/GA/GA_color_space.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BD19"/>
+  <dimension ref="A1:BV19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -714,6 +714,96 @@
           <t>xyz_z_75</t>
         </is>
       </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>yuv_y_mean</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>yuv_y_median</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>yuv_y_variance</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>yuv_y_std_dev</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>yuv_y_25</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>yuv_y_75</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>yuv_u_mean</t>
+        </is>
+      </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>yuv_u_median</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
+        <is>
+          <t>yuv_u_variance</t>
+        </is>
+      </c>
+      <c r="BN1" s="1" t="inlineStr">
+        <is>
+          <t>yuv_u_std_dev</t>
+        </is>
+      </c>
+      <c r="BO1" s="1" t="inlineStr">
+        <is>
+          <t>yuv_u_25</t>
+        </is>
+      </c>
+      <c r="BP1" s="1" t="inlineStr">
+        <is>
+          <t>yuv_u_75</t>
+        </is>
+      </c>
+      <c r="BQ1" s="1" t="inlineStr">
+        <is>
+          <t>yuv_v_mean</t>
+        </is>
+      </c>
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>yuv_v_median</t>
+        </is>
+      </c>
+      <c r="BS1" s="1" t="inlineStr">
+        <is>
+          <t>yuv_v_variance</t>
+        </is>
+      </c>
+      <c r="BT1" s="1" t="inlineStr">
+        <is>
+          <t>yuv_v_std_dev</t>
+        </is>
+      </c>
+      <c r="BU1" s="1" t="inlineStr">
+        <is>
+          <t>yuv_v_25</t>
+        </is>
+      </c>
+      <c r="BV1" s="1" t="inlineStr">
+        <is>
+          <t>yuv_v_75</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -996,6 +1086,96 @@
           <t>157.0</t>
         </is>
       </c>
+      <c r="BE2" t="inlineStr">
+        <is>
+          <t>164.8959850843257</t>
+        </is>
+      </c>
+      <c r="BF2" t="inlineStr">
+        <is>
+          <t>170.0</t>
+        </is>
+      </c>
+      <c r="BG2" t="inlineStr">
+        <is>
+          <t>613.2283322755437</t>
+        </is>
+      </c>
+      <c r="BH2" t="inlineStr">
+        <is>
+          <t>24.763447503842105</t>
+        </is>
+      </c>
+      <c r="BI2" t="inlineStr">
+        <is>
+          <t>152.0</t>
+        </is>
+      </c>
+      <c r="BJ2" t="inlineStr">
+        <is>
+          <t>182.0</t>
+        </is>
+      </c>
+      <c r="BK2" t="inlineStr">
+        <is>
+          <t>124.37258847554524</t>
+        </is>
+      </c>
+      <c r="BL2" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BM2" t="inlineStr">
+        <is>
+          <t>73.07829577324392</t>
+        </is>
+      </c>
+      <c r="BN2" t="inlineStr">
+        <is>
+          <t>8.548584430959545</t>
+        </is>
+      </c>
+      <c r="BO2" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BP2" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BQ2" t="inlineStr">
+        <is>
+          <t>131.0718037287394</t>
+        </is>
+      </c>
+      <c r="BR2" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BS2" t="inlineStr">
+        <is>
+          <t>50.01187780150411</t>
+        </is>
+      </c>
+      <c r="BT2" t="inlineStr">
+        <is>
+          <t>7.071907649390234</t>
+        </is>
+      </c>
+      <c r="BU2" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BV2" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1278,6 +1458,96 @@
           <t>43.0</t>
         </is>
       </c>
+      <c r="BE3" t="inlineStr">
+        <is>
+          <t>69.82749431715365</t>
+        </is>
+      </c>
+      <c r="BF3" t="inlineStr">
+        <is>
+          <t>62.0</t>
+        </is>
+      </c>
+      <c r="BG3" t="inlineStr">
+        <is>
+          <t>1131.7800864375947</t>
+        </is>
+      </c>
+      <c r="BH3" t="inlineStr">
+        <is>
+          <t>33.64193939768626</t>
+        </is>
+      </c>
+      <c r="BI3" t="inlineStr">
+        <is>
+          <t>47.0</t>
+        </is>
+      </c>
+      <c r="BJ3" t="inlineStr">
+        <is>
+          <t>86.0</t>
+        </is>
+      </c>
+      <c r="BK3" t="inlineStr">
+        <is>
+          <t>119.17062670095316</t>
+        </is>
+      </c>
+      <c r="BL3" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BM3" t="inlineStr">
+        <is>
+          <t>140.86831254136672</t>
+        </is>
+      </c>
+      <c r="BN3" t="inlineStr">
+        <is>
+          <t>11.868795749416481</t>
+        </is>
+      </c>
+      <c r="BO3" t="inlineStr">
+        <is>
+          <t>109.0</t>
+        </is>
+      </c>
+      <c r="BP3" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BQ3" t="inlineStr">
+        <is>
+          <t>139.8080439194962</t>
+        </is>
+      </c>
+      <c r="BR3" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BS3" t="inlineStr">
+        <is>
+          <t>235.62295702171465</t>
+        </is>
+      </c>
+      <c r="BT3" t="inlineStr">
+        <is>
+          <t>15.350014886693584</t>
+        </is>
+      </c>
+      <c r="BU3" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BV3" t="inlineStr">
+        <is>
+          <t>153.0</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1560,6 +1830,96 @@
           <t>153.0</t>
         </is>
       </c>
+      <c r="BE4" t="inlineStr">
+        <is>
+          <t>157.3742395636669</t>
+        </is>
+      </c>
+      <c r="BF4" t="inlineStr">
+        <is>
+          <t>158.0</t>
+        </is>
+      </c>
+      <c r="BG4" t="inlineStr">
+        <is>
+          <t>603.0285125064859</t>
+        </is>
+      </c>
+      <c r="BH4" t="inlineStr">
+        <is>
+          <t>24.556638868267086</t>
+        </is>
+      </c>
+      <c r="BI4" t="inlineStr">
+        <is>
+          <t>144.0</t>
+        </is>
+      </c>
+      <c r="BJ4" t="inlineStr">
+        <is>
+          <t>171.0</t>
+        </is>
+      </c>
+      <c r="BK4" t="inlineStr">
+        <is>
+          <t>126.23806349436443</t>
+        </is>
+      </c>
+      <c r="BL4" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BM4" t="inlineStr">
+        <is>
+          <t>39.12484782414402</t>
+        </is>
+      </c>
+      <c r="BN4" t="inlineStr">
+        <is>
+          <t>6.254985837245679</t>
+        </is>
+      </c>
+      <c r="BO4" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BP4" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BQ4" t="inlineStr">
+        <is>
+          <t>129.79143555959067</t>
+        </is>
+      </c>
+      <c r="BR4" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BS4" t="inlineStr">
+        <is>
+          <t>33.31207421048003</t>
+        </is>
+      </c>
+      <c r="BT4" t="inlineStr">
+        <is>
+          <t>5.7716613042069635</t>
+        </is>
+      </c>
+      <c r="BU4" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BV4" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1842,6 +2202,96 @@
           <t>53.0</t>
         </is>
       </c>
+      <c r="BE5" t="inlineStr">
+        <is>
+          <t>65.32000986781715</t>
+        </is>
+      </c>
+      <c r="BF5" t="inlineStr">
+        <is>
+          <t>54.0</t>
+        </is>
+      </c>
+      <c r="BG5" t="inlineStr">
+        <is>
+          <t>1554.6748563979202</t>
+        </is>
+      </c>
+      <c r="BH5" t="inlineStr">
+        <is>
+          <t>39.42936540698975</t>
+        </is>
+      </c>
+      <c r="BI5" t="inlineStr">
+        <is>
+          <t>38.0</t>
+        </is>
+      </c>
+      <c r="BJ5" t="inlineStr">
+        <is>
+          <t>86.0</t>
+        </is>
+      </c>
+      <c r="BK5" t="inlineStr">
+        <is>
+          <t>126.088028271993</t>
+        </is>
+      </c>
+      <c r="BL5" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BM5" t="inlineStr">
+        <is>
+          <t>36.091717665073695</t>
+        </is>
+      </c>
+      <c r="BN5" t="inlineStr">
+        <is>
+          <t>6.007638276816747</t>
+        </is>
+      </c>
+      <c r="BO5" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BP5" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BQ5" t="inlineStr">
+        <is>
+          <t>130.97281392415366</t>
+        </is>
+      </c>
+      <c r="BR5" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BS5" t="inlineStr">
+        <is>
+          <t>82.59342989819632</t>
+        </is>
+      </c>
+      <c r="BT5" t="inlineStr">
+        <is>
+          <t>9.088092753608775</t>
+        </is>
+      </c>
+      <c r="BU5" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BV5" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2124,6 +2574,96 @@
           <t>121.0</t>
         </is>
       </c>
+      <c r="BE6" t="inlineStr">
+        <is>
+          <t>127.9930184696415</t>
+        </is>
+      </c>
+      <c r="BF6" t="inlineStr">
+        <is>
+          <t>121.0</t>
+        </is>
+      </c>
+      <c r="BG6" t="inlineStr">
+        <is>
+          <t>1474.2380220306354</t>
+        </is>
+      </c>
+      <c r="BH6" t="inlineStr">
+        <is>
+          <t>38.39580734963956</t>
+        </is>
+      </c>
+      <c r="BI6" t="inlineStr">
+        <is>
+          <t>94.0</t>
+        </is>
+      </c>
+      <c r="BJ6" t="inlineStr">
+        <is>
+          <t>164.0</t>
+        </is>
+      </c>
+      <c r="BK6" t="inlineStr">
+        <is>
+          <t>116.37011528384502</t>
+        </is>
+      </c>
+      <c r="BL6" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BM6" t="inlineStr">
+        <is>
+          <t>224.3214711505171</t>
+        </is>
+      </c>
+      <c r="BN6" t="inlineStr">
+        <is>
+          <t>14.977365294020077</t>
+        </is>
+      </c>
+      <c r="BO6" t="inlineStr">
+        <is>
+          <t>104.0</t>
+        </is>
+      </c>
+      <c r="BP6" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BQ6" t="inlineStr">
+        <is>
+          <t>139.64912215582197</t>
+        </is>
+      </c>
+      <c r="BR6" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BS6" t="inlineStr">
+        <is>
+          <t>214.48752305540023</t>
+        </is>
+      </c>
+      <c r="BT6" t="inlineStr">
+        <is>
+          <t>14.64539255381706</t>
+        </is>
+      </c>
+      <c r="BU6" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BV6" t="inlineStr">
+        <is>
+          <t>153.0</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2406,6 +2946,96 @@
           <t>161.0</t>
         </is>
       </c>
+      <c r="BE7" t="inlineStr">
+        <is>
+          <t>154.90508266705513</t>
+        </is>
+      </c>
+      <c r="BF7" t="inlineStr">
+        <is>
+          <t>159.0</t>
+        </is>
+      </c>
+      <c r="BG7" t="inlineStr">
+        <is>
+          <t>783.8468467039286</t>
+        </is>
+      </c>
+      <c r="BH7" t="inlineStr">
+        <is>
+          <t>27.99726498613621</t>
+        </is>
+      </c>
+      <c r="BI7" t="inlineStr">
+        <is>
+          <t>139.0</t>
+        </is>
+      </c>
+      <c r="BJ7" t="inlineStr">
+        <is>
+          <t>176.0</t>
+        </is>
+      </c>
+      <c r="BK7" t="inlineStr">
+        <is>
+          <t>117.89861506163642</t>
+        </is>
+      </c>
+      <c r="BL7" t="inlineStr">
+        <is>
+          <t>121.0</t>
+        </is>
+      </c>
+      <c r="BM7" t="inlineStr">
+        <is>
+          <t>144.98038497165638</t>
+        </is>
+      </c>
+      <c r="BN7" t="inlineStr">
+        <is>
+          <t>12.040780081525298</t>
+        </is>
+      </c>
+      <c r="BO7" t="inlineStr">
+        <is>
+          <t>110.0</t>
+        </is>
+      </c>
+      <c r="BP7" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BQ7" t="inlineStr">
+        <is>
+          <t>138.1891388170051</t>
+        </is>
+      </c>
+      <c r="BR7" t="inlineStr">
+        <is>
+          <t>141.0</t>
+        </is>
+      </c>
+      <c r="BS7" t="inlineStr">
+        <is>
+          <t>111.7593856376652</t>
+        </is>
+      </c>
+      <c r="BT7" t="inlineStr">
+        <is>
+          <t>10.571631172040822</t>
+        </is>
+      </c>
+      <c r="BU7" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BV7" t="inlineStr">
+        <is>
+          <t>146.0</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2688,6 +3318,96 @@
           <t>50.0</t>
         </is>
       </c>
+      <c r="BE8" t="inlineStr">
+        <is>
+          <t>69.97129509581187</t>
+        </is>
+      </c>
+      <c r="BF8" t="inlineStr">
+        <is>
+          <t>63.0</t>
+        </is>
+      </c>
+      <c r="BG8" t="inlineStr">
+        <is>
+          <t>1205.8532785132802</t>
+        </is>
+      </c>
+      <c r="BH8" t="inlineStr">
+        <is>
+          <t>34.72539817645408</t>
+        </is>
+      </c>
+      <c r="BI8" t="inlineStr">
+        <is>
+          <t>47.0</t>
+        </is>
+      </c>
+      <c r="BJ8" t="inlineStr">
+        <is>
+          <t>85.0</t>
+        </is>
+      </c>
+      <c r="BK8" t="inlineStr">
+        <is>
+          <t>119.18571914064259</t>
+        </is>
+      </c>
+      <c r="BL8" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BM8" t="inlineStr">
+        <is>
+          <t>130.6443139480517</t>
+        </is>
+      </c>
+      <c r="BN8" t="inlineStr">
+        <is>
+          <t>11.429974363403081</t>
+        </is>
+      </c>
+      <c r="BO8" t="inlineStr">
+        <is>
+          <t>111.0</t>
+        </is>
+      </c>
+      <c r="BP8" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BQ8" t="inlineStr">
+        <is>
+          <t>141.4154584426911</t>
+        </is>
+      </c>
+      <c r="BR8" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BS8" t="inlineStr">
+        <is>
+          <t>275.55253339364066</t>
+        </is>
+      </c>
+      <c r="BT8" t="inlineStr">
+        <is>
+          <t>16.599775100694607</t>
+        </is>
+      </c>
+      <c r="BU8" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BV8" t="inlineStr">
+        <is>
+          <t>155.0</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2970,6 +3690,96 @@
           <t>138.0</t>
         </is>
       </c>
+      <c r="BE9" t="inlineStr">
+        <is>
+          <t>149.80062564990328</t>
+        </is>
+      </c>
+      <c r="BF9" t="inlineStr">
+        <is>
+          <t>149.0</t>
+        </is>
+      </c>
+      <c r="BG9" t="inlineStr">
+        <is>
+          <t>681.7126418030423</t>
+        </is>
+      </c>
+      <c r="BH9" t="inlineStr">
+        <is>
+          <t>26.109627377713423</t>
+        </is>
+      </c>
+      <c r="BI9" t="inlineStr">
+        <is>
+          <t>130.0</t>
+        </is>
+      </c>
+      <c r="BJ9" t="inlineStr">
+        <is>
+          <t>168.0</t>
+        </is>
+      </c>
+      <c r="BK9" t="inlineStr">
+        <is>
+          <t>125.31965573628743</t>
+        </is>
+      </c>
+      <c r="BL9" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BM9" t="inlineStr">
+        <is>
+          <t>79.29437642872357</t>
+        </is>
+      </c>
+      <c r="BN9" t="inlineStr">
+        <is>
+          <t>8.904738987119362</t>
+        </is>
+      </c>
+      <c r="BO9" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BP9" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BQ9" t="inlineStr">
+        <is>
+          <t>130.57684739430746</t>
+        </is>
+      </c>
+      <c r="BR9" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BS9" t="inlineStr">
+        <is>
+          <t>59.85146358300949</t>
+        </is>
+      </c>
+      <c r="BT9" t="inlineStr">
+        <is>
+          <t>7.736372766549547</t>
+        </is>
+      </c>
+      <c r="BU9" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BV9" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -3252,6 +4062,96 @@
           <t>34.0</t>
         </is>
       </c>
+      <c r="BE10" t="inlineStr">
+        <is>
+          <t>71.54639323103399</t>
+        </is>
+      </c>
+      <c r="BF10" t="inlineStr">
+        <is>
+          <t>66.0</t>
+        </is>
+      </c>
+      <c r="BG10" t="inlineStr">
+        <is>
+          <t>1272.6066192564858</t>
+        </is>
+      </c>
+      <c r="BH10" t="inlineStr">
+        <is>
+          <t>35.67361236623628</t>
+        </is>
+      </c>
+      <c r="BI10" t="inlineStr">
+        <is>
+          <t>47.0</t>
+        </is>
+      </c>
+      <c r="BJ10" t="inlineStr">
+        <is>
+          <t>90.0</t>
+        </is>
+      </c>
+      <c r="BK10" t="inlineStr">
+        <is>
+          <t>118.00927904678507</t>
+        </is>
+      </c>
+      <c r="BL10" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BM10" t="inlineStr">
+        <is>
+          <t>191.68644003804525</t>
+        </is>
+      </c>
+      <c r="BN10" t="inlineStr">
+        <is>
+          <t>13.84508721670056</t>
+        </is>
+      </c>
+      <c r="BO10" t="inlineStr">
+        <is>
+          <t>106.0</t>
+        </is>
+      </c>
+      <c r="BP10" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BQ10" t="inlineStr">
+        <is>
+          <t>142.47142374727488</t>
+        </is>
+      </c>
+      <c r="BR10" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BS10" t="inlineStr">
+        <is>
+          <t>382.76222173726865</t>
+        </is>
+      </c>
+      <c r="BT10" t="inlineStr">
+        <is>
+          <t>19.564309896780635</t>
+        </is>
+      </c>
+      <c r="BU10" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BV10" t="inlineStr">
+        <is>
+          <t>159.0</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -3534,6 +4434,96 @@
           <t>124.0</t>
         </is>
       </c>
+      <c r="BE11" t="inlineStr">
+        <is>
+          <t>137.06397578462682</t>
+        </is>
+      </c>
+      <c r="BF11" t="inlineStr">
+        <is>
+          <t>137.0</t>
+        </is>
+      </c>
+      <c r="BG11" t="inlineStr">
+        <is>
+          <t>888.5537392587412</t>
+        </is>
+      </c>
+      <c r="BH11" t="inlineStr">
+        <is>
+          <t>29.808618539924677</t>
+        </is>
+      </c>
+      <c r="BI11" t="inlineStr">
+        <is>
+          <t>114.0</t>
+        </is>
+      </c>
+      <c r="BJ11" t="inlineStr">
+        <is>
+          <t>160.0</t>
+        </is>
+      </c>
+      <c r="BK11" t="inlineStr">
+        <is>
+          <t>116.28261351052049</t>
+        </is>
+      </c>
+      <c r="BL11" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BM11" t="inlineStr">
+        <is>
+          <t>219.78683318432832</t>
+        </is>
+      </c>
+      <c r="BN11" t="inlineStr">
+        <is>
+          <t>14.825209380792176</t>
+        </is>
+      </c>
+      <c r="BO11" t="inlineStr">
+        <is>
+          <t>104.0</t>
+        </is>
+      </c>
+      <c r="BP11" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BQ11" t="inlineStr">
+        <is>
+          <t>139.24455944572225</t>
+        </is>
+      </c>
+      <c r="BR11" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BS11" t="inlineStr">
+        <is>
+          <t>185.15431595791244</t>
+        </is>
+      </c>
+      <c r="BT11" t="inlineStr">
+        <is>
+          <t>13.60714209369155</t>
+        </is>
+      </c>
+      <c r="BU11" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BV11" t="inlineStr">
+        <is>
+          <t>152.0</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -3816,6 +4806,96 @@
           <t>150.0</t>
         </is>
       </c>
+      <c r="BE12" t="inlineStr">
+        <is>
+          <t>154.17888870252503</t>
+        </is>
+      </c>
+      <c r="BF12" t="inlineStr">
+        <is>
+          <t>154.0</t>
+        </is>
+      </c>
+      <c r="BG12" t="inlineStr">
+        <is>
+          <t>669.1862034419659</t>
+        </is>
+      </c>
+      <c r="BH12" t="inlineStr">
+        <is>
+          <t>25.868633582815423</t>
+        </is>
+      </c>
+      <c r="BI12" t="inlineStr">
+        <is>
+          <t>134.0</t>
+        </is>
+      </c>
+      <c r="BJ12" t="inlineStr">
+        <is>
+          <t>172.0</t>
+        </is>
+      </c>
+      <c r="BK12" t="inlineStr">
+        <is>
+          <t>125.8896697362264</t>
+        </is>
+      </c>
+      <c r="BL12" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BM12" t="inlineStr">
+        <is>
+          <t>45.33790740511649</t>
+        </is>
+      </c>
+      <c r="BN12" t="inlineStr">
+        <is>
+          <t>6.733342959118931</t>
+        </is>
+      </c>
+      <c r="BO12" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BP12" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BQ12" t="inlineStr">
+        <is>
+          <t>130.12718645731607</t>
+        </is>
+      </c>
+      <c r="BR12" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BS12" t="inlineStr">
+        <is>
+          <t>41.322547741428004</t>
+        </is>
+      </c>
+      <c r="BT12" t="inlineStr">
+        <is>
+          <t>6.428261642265971</t>
+        </is>
+      </c>
+      <c r="BU12" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BV12" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -4098,6 +5178,96 @@
           <t>144.0</t>
         </is>
       </c>
+      <c r="BE13" t="inlineStr">
+        <is>
+          <t>157.72130242287182</t>
+        </is>
+      </c>
+      <c r="BF13" t="inlineStr">
+        <is>
+          <t>153.0</t>
+        </is>
+      </c>
+      <c r="BG13" t="inlineStr">
+        <is>
+          <t>627.2485987559955</t>
+        </is>
+      </c>
+      <c r="BH13" t="inlineStr">
+        <is>
+          <t>25.044931598149667</t>
+        </is>
+      </c>
+      <c r="BI13" t="inlineStr">
+        <is>
+          <t>140.0</t>
+        </is>
+      </c>
+      <c r="BJ13" t="inlineStr">
+        <is>
+          <t>177.0</t>
+        </is>
+      </c>
+      <c r="BK13" t="inlineStr">
+        <is>
+          <t>124.4005651473999</t>
+        </is>
+      </c>
+      <c r="BL13" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BM13" t="inlineStr">
+        <is>
+          <t>77.60302075553871</t>
+        </is>
+      </c>
+      <c r="BN13" t="inlineStr">
+        <is>
+          <t>8.809257673353567</t>
+        </is>
+      </c>
+      <c r="BO13" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BP13" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BQ13" t="inlineStr">
+        <is>
+          <t>131.3976256052653</t>
+        </is>
+      </c>
+      <c r="BR13" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BS13" t="inlineStr">
+        <is>
+          <t>64.62705076382015</t>
+        </is>
+      </c>
+      <c r="BT13" t="inlineStr">
+        <is>
+          <t>8.039095145837008</t>
+        </is>
+      </c>
+      <c r="BU13" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BV13" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -4380,6 +5550,96 @@
           <t>44.0</t>
         </is>
       </c>
+      <c r="BE14" t="inlineStr">
+        <is>
+          <t>72.8213667040417</t>
+        </is>
+      </c>
+      <c r="BF14" t="inlineStr">
+        <is>
+          <t>66.0</t>
+        </is>
+      </c>
+      <c r="BG14" t="inlineStr">
+        <is>
+          <t>1086.0849232686103</t>
+        </is>
+      </c>
+      <c r="BH14" t="inlineStr">
+        <is>
+          <t>32.955802573577394</t>
+        </is>
+      </c>
+      <c r="BI14" t="inlineStr">
+        <is>
+          <t>48.0</t>
+        </is>
+      </c>
+      <c r="BJ14" t="inlineStr">
+        <is>
+          <t>90.0</t>
+        </is>
+      </c>
+      <c r="BK14" t="inlineStr">
+        <is>
+          <t>125.63858032226562</t>
+        </is>
+      </c>
+      <c r="BL14" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BM14" t="inlineStr">
+        <is>
+          <t>56.476498873593904</t>
+        </is>
+      </c>
+      <c r="BN14" t="inlineStr">
+        <is>
+          <t>7.515084754917532</t>
+        </is>
+      </c>
+      <c r="BO14" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BP14" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BQ14" t="inlineStr">
+        <is>
+          <t>131.14692974090576</t>
+        </is>
+      </c>
+      <c r="BR14" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BS14" t="inlineStr">
+        <is>
+          <t>93.63746895053286</t>
+        </is>
+      </c>
+      <c r="BT14" t="inlineStr">
+        <is>
+          <t>9.676645542259614</t>
+        </is>
+      </c>
+      <c r="BU14" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BV14" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -4662,6 +5922,96 @@
           <t>152.0</t>
         </is>
       </c>
+      <c r="BE15" t="inlineStr">
+        <is>
+          <t>156.58526826545528</t>
+        </is>
+      </c>
+      <c r="BF15" t="inlineStr">
+        <is>
+          <t>159.0</t>
+        </is>
+      </c>
+      <c r="BG15" t="inlineStr">
+        <is>
+          <t>807.3982340355473</t>
+        </is>
+      </c>
+      <c r="BH15" t="inlineStr">
+        <is>
+          <t>28.41475380916659</t>
+        </is>
+      </c>
+      <c r="BI15" t="inlineStr">
+        <is>
+          <t>133.0</t>
+        </is>
+      </c>
+      <c r="BJ15" t="inlineStr">
+        <is>
+          <t>178.0</t>
+        </is>
+      </c>
+      <c r="BK15" t="inlineStr">
+        <is>
+          <t>116.57392084958916</t>
+        </is>
+      </c>
+      <c r="BL15" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BM15" t="inlineStr">
+        <is>
+          <t>201.11730439220088</t>
+        </is>
+      </c>
+      <c r="BN15" t="inlineStr">
+        <is>
+          <t>14.181583282278494</t>
+        </is>
+      </c>
+      <c r="BO15" t="inlineStr">
+        <is>
+          <t>107.0</t>
+        </is>
+      </c>
+      <c r="BP15" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BQ15" t="inlineStr">
+        <is>
+          <t>139.28720358100304</t>
+        </is>
+      </c>
+      <c r="BR15" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BS15" t="inlineStr">
+        <is>
+          <t>151.6190122722358</t>
+        </is>
+      </c>
+      <c r="BT15" t="inlineStr">
+        <is>
+          <t>12.31336721909307</t>
+        </is>
+      </c>
+      <c r="BU15" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BV15" t="inlineStr">
+        <is>
+          <t>151.0</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -4944,6 +6294,96 @@
           <t>119.0</t>
         </is>
       </c>
+      <c r="BE16" t="inlineStr">
+        <is>
+          <t>135.03407748686826</t>
+        </is>
+      </c>
+      <c r="BF16" t="inlineStr">
+        <is>
+          <t>132.0</t>
+        </is>
+      </c>
+      <c r="BG16" t="inlineStr">
+        <is>
+          <t>1133.3738415948674</t>
+        </is>
+      </c>
+      <c r="BH16" t="inlineStr">
+        <is>
+          <t>33.66561809316543</t>
+        </is>
+      </c>
+      <c r="BI16" t="inlineStr">
+        <is>
+          <t>106.0</t>
+        </is>
+      </c>
+      <c r="BJ16" t="inlineStr">
+        <is>
+          <t>162.0</t>
+        </is>
+      </c>
+      <c r="BK16" t="inlineStr">
+        <is>
+          <t>124.39188925425212</t>
+        </is>
+      </c>
+      <c r="BL16" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BM16" t="inlineStr">
+        <is>
+          <t>105.67321235046732</t>
+        </is>
+      </c>
+      <c r="BN16" t="inlineStr">
+        <is>
+          <t>10.279747679319144</t>
+        </is>
+      </c>
+      <c r="BO16" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BP16" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BQ16" t="inlineStr">
+        <is>
+          <t>131.52151997884116</t>
+        </is>
+      </c>
+      <c r="BR16" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BS16" t="inlineStr">
+        <is>
+          <t>97.3456570890782</t>
+        </is>
+      </c>
+      <c r="BT16" t="inlineStr">
+        <is>
+          <t>9.866390276543807</t>
+        </is>
+      </c>
+      <c r="BU16" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BV16" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -5226,6 +6666,96 @@
           <t>143.0</t>
         </is>
       </c>
+      <c r="BE17" t="inlineStr">
+        <is>
+          <t>151.3998498170306</t>
+        </is>
+      </c>
+      <c r="BF17" t="inlineStr">
+        <is>
+          <t>152.0</t>
+        </is>
+      </c>
+      <c r="BG17" t="inlineStr">
+        <is>
+          <t>670.68821322316</t>
+        </is>
+      </c>
+      <c r="BH17" t="inlineStr">
+        <is>
+          <t>25.897648797200876</t>
+        </is>
+      </c>
+      <c r="BI17" t="inlineStr">
+        <is>
+          <t>132.0</t>
+        </is>
+      </c>
+      <c r="BJ17" t="inlineStr">
+        <is>
+          <t>172.0</t>
+        </is>
+      </c>
+      <c r="BK17" t="inlineStr">
+        <is>
+          <t>126.04481919606526</t>
+        </is>
+      </c>
+      <c r="BL17" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BM17" t="inlineStr">
+        <is>
+          <t>46.60446166558746</t>
+        </is>
+      </c>
+      <c r="BN17" t="inlineStr">
+        <is>
+          <t>6.826746052519272</t>
+        </is>
+      </c>
+      <c r="BO17" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BP17" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BQ17" t="inlineStr">
+        <is>
+          <t>129.63724835713705</t>
+        </is>
+      </c>
+      <c r="BR17" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BS17" t="inlineStr">
+        <is>
+          <t>30.79283573493937</t>
+        </is>
+      </c>
+      <c r="BT17" t="inlineStr">
+        <is>
+          <t>5.549129277187491</t>
+        </is>
+      </c>
+      <c r="BU17" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BV17" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -5508,6 +7038,96 @@
           <t>103.0</t>
         </is>
       </c>
+      <c r="BE18" t="inlineStr">
+        <is>
+          <t>117.45208119562793</t>
+        </is>
+      </c>
+      <c r="BF18" t="inlineStr">
+        <is>
+          <t>117.0</t>
+        </is>
+      </c>
+      <c r="BG18" t="inlineStr">
+        <is>
+          <t>780.2514096399237</t>
+        </is>
+      </c>
+      <c r="BH18" t="inlineStr">
+        <is>
+          <t>27.932980679475</t>
+        </is>
+      </c>
+      <c r="BI18" t="inlineStr">
+        <is>
+          <t>96.0</t>
+        </is>
+      </c>
+      <c r="BJ18" t="inlineStr">
+        <is>
+          <t>136.0</t>
+        </is>
+      </c>
+      <c r="BK18" t="inlineStr">
+        <is>
+          <t>125.48865667978923</t>
+        </is>
+      </c>
+      <c r="BL18" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BM18" t="inlineStr">
+        <is>
+          <t>64.01310769281541</t>
+        </is>
+      </c>
+      <c r="BN18" t="inlineStr">
+        <is>
+          <t>8.000819188859063</t>
+        </is>
+      </c>
+      <c r="BO18" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BP18" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BQ18" t="inlineStr">
+        <is>
+          <t>130.53190898895264</t>
+        </is>
+      </c>
+      <c r="BR18" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BS18" t="inlineStr">
+        <is>
+          <t>58.84541545595001</t>
+        </is>
+      </c>
+      <c r="BT18" t="inlineStr">
+        <is>
+          <t>7.671076551302953</t>
+        </is>
+      </c>
+      <c r="BU18" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BV18" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -5788,6 +7408,96 @@
       <c r="BD19" t="inlineStr">
         <is>
           <t>86.0</t>
+        </is>
+      </c>
+      <c r="BE19" t="inlineStr">
+        <is>
+          <t>88.8200859235754</t>
+        </is>
+      </c>
+      <c r="BF19" t="inlineStr">
+        <is>
+          <t>90.0</t>
+        </is>
+      </c>
+      <c r="BG19" t="inlineStr">
+        <is>
+          <t>826.5811705849128</t>
+        </is>
+      </c>
+      <c r="BH19" t="inlineStr">
+        <is>
+          <t>28.75032470399096</t>
+        </is>
+      </c>
+      <c r="BI19" t="inlineStr">
+        <is>
+          <t>65.0</t>
+        </is>
+      </c>
+      <c r="BJ19" t="inlineStr">
+        <is>
+          <t>110.0</t>
+        </is>
+      </c>
+      <c r="BK19" t="inlineStr">
+        <is>
+          <t>116.8296035844991</t>
+        </is>
+      </c>
+      <c r="BL19" t="inlineStr">
+        <is>
+          <t>118.0</t>
+        </is>
+      </c>
+      <c r="BM19" t="inlineStr">
+        <is>
+          <t>141.7173508056759</t>
+        </is>
+      </c>
+      <c r="BN19" t="inlineStr">
+        <is>
+          <t>11.904509683547488</t>
+        </is>
+      </c>
+      <c r="BO19" t="inlineStr">
+        <is>
+          <t>107.0</t>
+        </is>
+      </c>
+      <c r="BP19" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BQ19" t="inlineStr">
+        <is>
+          <t>141.70834627355748</t>
+        </is>
+      </c>
+      <c r="BR19" t="inlineStr">
+        <is>
+          <t>143.0</t>
+        </is>
+      </c>
+      <c r="BS19" t="inlineStr">
+        <is>
+          <t>200.00484472901897</t>
+        </is>
+      </c>
+      <c r="BT19" t="inlineStr">
+        <is>
+          <t>14.142306909730781</t>
+        </is>
+      </c>
+      <c r="BU19" t="inlineStr">
+        <is>
+          <t>128.0</t>
+        </is>
+      </c>
+      <c r="BV19" t="inlineStr">
+        <is>
+          <t>154.0</t>
         </is>
       </c>
     </row>

</xml_diff>